<commit_message>
20 formatacao condicional primeiros/ultimos
</commit_message>
<xml_diff>
--- a/005-formatacao/20-formatacaoCondicional-primeirosUltimos.xlsx
+++ b/005-formatacao/20-formatacaoCondicional-primeirosUltimos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaof\Desktop\Excel Imp\Módulo 3 - Formatação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jorge\Desktop\hashtag\hashtagExcel\005-formatacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A3DD248-26B8-49F0-AB55-F2CC30131A3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{635149F7-4745-4844-A04D-F09DBC6F2475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{60DE4CDD-BFE8-488F-B25C-A1E3AA20DCD1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{60DE4CDD-BFE8-488F-B25C-A1E3AA20DCD1}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="&quot;R$&quot;\ #,##0"/>
+    <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -215,16 +215,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -235,138 +234,246 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF8181"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9393"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+  <dxfs count="24">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -391,7 +498,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -690,17 +797,17 @@
   <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="15.44140625" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.5546875" customWidth="1"/>
+    <col min="1" max="4" width="15.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -713,250 +820,250 @@
       <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="H1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>35000</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>5000000</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>45000</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>1000000</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="6" t="s">
         <v>27</v>
       </c>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>135175</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>3784900</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>28</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>7418</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>207704</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>71371</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>2212501</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
+        <v>130000</v>
+      </c>
+      <c r="D7" s="5">
         <v>0</v>
       </c>
-      <c r="D7" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>145414</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>4217006</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>28010</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>942462</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>30523</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>732552</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>0</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="5">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>47498</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="5">
         <v>1187450</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>3</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>22285</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>668550</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>71711</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>1936197</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>25000</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>2200125</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>127481</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="5">
         <v>2677101</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>5000</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="5">
         <v>3000000</v>
       </c>
     </row>
@@ -970,6 +1077,13 @@
     <mergeCell ref="G1:H1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C2:C17">
+    <cfRule type="top10" dxfId="4" priority="3" percent="1" rank="30"/>
+    <cfRule type="top10" dxfId="3" priority="2" percent="1" bottom="1" rank="30"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D2:D17">
+    <cfRule type="aboveAverage" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>